<commit_message>
Update Porkjet radiator rebalance.xlsx
</commit_message>
<xml_diff>
--- a/Porkjet radiator rebalance.xlsx
+++ b/Porkjet radiator rebalance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19470" windowHeight="8340"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19470" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Rads</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Heat Control EF-2k square graphene</t>
   </si>
   <si>
-    <t>EC demand</t>
-  </si>
-  <si>
     <t>EC req</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>exp cost</t>
+  </si>
+  <si>
+    <t>EC Demand</t>
   </si>
 </sst>
 </file>
@@ -100,9 +100,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="169" formatCode="0.000"/>
-    <numFmt numFmtId="173" formatCode="0\ &quot;kW&quot;"/>
-    <numFmt numFmtId="175" formatCode="0.000\ &quot;t&quot;"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0\ &quot;kW&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.000\ &quot;t&quot;"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -135,12 +135,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -165,19 +171,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -461,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,10 +507,10 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -606,21 +620,25 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -636,28 +654,34 @@
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="11">
         <v>100</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="12">
         <f>D2</f>
         <v>226.38126707264092</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="13">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="14">
         <f>E2</f>
         <v>6.0500000000000012E-2</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G13" s="16">
         <f>F2</f>
         <v>2.8297658384080118E-2</v>
       </c>
@@ -666,135 +690,157 @@
       <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>150</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7">
+      <c r="C14" s="5"/>
+      <c r="D14" s="6">
         <v>0.12</v>
       </c>
-      <c r="E14" s="8"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="17">
+        <v>3.7999999999999999E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="11">
         <v>200</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="12">
         <f>D3</f>
         <v>624.17247043552152</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="13">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="14">
         <f>E3</f>
         <v>0.28799999999999998</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G16" s="16">
         <f>F3</f>
         <v>7.8021558804440186E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>75</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7">
+      <c r="C17" s="5"/>
+      <c r="D17" s="6">
         <v>0.06</v>
       </c>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="E17" s="7"/>
+      <c r="F17" s="17">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="11">
         <v>500</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="12">
         <f>D4</f>
         <v>1921.6191056317521</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="13">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="14">
         <f>E4</f>
         <v>1.6245000000000003</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G19" s="16">
         <f>F4</f>
         <v>0.240202388203969</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>150</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7">
+      <c r="C20" s="5"/>
+      <c r="D20" s="6">
         <v>0.12</v>
       </c>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="E20" s="7"/>
+      <c r="F20" s="17">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>2000</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7">
+      <c r="C21" s="5"/>
+      <c r="D21" s="6">
         <v>1.244</v>
       </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="E21" s="7"/>
+      <c r="F21" s="17">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>200</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>0.05</v>
       </c>
+      <c r="F23" s="17">
+        <v>2.5000000000000001E-2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>